<commit_message>
so sanh dang nv
</commit_message>
<xml_diff>
--- a/so_sanh_input.xlsx
+++ b/so_sanh_input.xlsx
@@ -1,12 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44038143-E8C9-47B5-84E8-0A799094D4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Input_Asset" state="visible" r:id="rId4"/>
-    <sheet sheetId="2" name="Input_Task" state="visible" r:id="rId5"/>
-    <sheet sheetId="3" name="Input_Employee" state="visible" r:id="rId6"/>
+    <sheet name="Input_Asset" sheetId="1" r:id="rId1"/>
+    <sheet name="Input_Task" sheetId="2" r:id="rId2"/>
+    <sheet name="Input_Employee" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -210,14 +214,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -580,11 +584,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="71.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -617,8 +629,11 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -631,8 +646,11 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -645,8 +663,11 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -659,11 +680,14 @@
       <c r="D5" t="s">
         <v>14</v>
       </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
       <c r="F5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -676,8 +700,11 @@
       <c r="D6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -690,19 +717,27 @@
       <c r="D7" t="s">
         <v>8</v>
       </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H15"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -728,7 +763,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -754,7 +789,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -780,7 +815,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -806,7 +841,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -832,7 +867,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -858,7 +893,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -884,7 +919,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -910,7 +945,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -936,7 +971,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -962,7 +997,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -988,7 +1023,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1014,7 +1049,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1040,7 +1075,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1066,7 +1101,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1094,16 +1129,34 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M5"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1144,7 +1197,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1185,7 +1238,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1226,7 +1279,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1267,7 +1320,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1310,6 +1363,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>